<commit_message>
updates to the raw and analyzed data and new draft figures
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryAnalysis_Dataset_v9.xlsx
+++ b/DataRe-Analysis/SummaryAnalysis_Dataset_v9.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="0" windowWidth="18480" windowHeight="16040" tabRatio="954" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1820" yWindow="0" windowWidth="26840" windowHeight="16040" tabRatio="954" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies-PRE" sheetId="15" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8478" uniqueCount="1541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8479" uniqueCount="1541">
   <si>
     <t>Organisms</t>
   </si>
@@ -5556,7 +5556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1156">
+  <cellStyleXfs count="1188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6288,6 +6288,38 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7370,21 +7402,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="1" xfId="150" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="9" borderId="1" xfId="150" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -7434,8 +7451,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="1" xfId="150" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="9" borderId="1" xfId="150" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1156">
+  <cellStyles count="1188">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -8375,6 +8407,22 @@
     <cellStyle name="Followed Hyperlink" xfId="1151" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1153" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1187" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
@@ -8587,6 +8635,22 @@
     <cellStyle name="Hyperlink" xfId="1150" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1152" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1186" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="150"/>
@@ -8749,11 +8813,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128803784"/>
-        <c:axId val="-2130583400"/>
+        <c:axId val="-2114375096"/>
+        <c:axId val="-2114372008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128803784"/>
+        <c:axId val="-2114375096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8776,7 +8840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130583400"/>
+        <c:crossAx val="-2114372008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8784,7 +8848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130583400"/>
+        <c:axId val="-2114372008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -8808,7 +8872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128803784"/>
+        <c:crossAx val="-2114375096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -8999,13 +9063,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.0148566094420601</c:v>
+                    <c:v>0.0182766094420601</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0562861151079137</c:v>
+                    <c:v>0.0599461151079137</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0774400000000001</c:v>
+                    <c:v>0.0650658415841584</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -9017,13 +9081,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.0235833905579399</c:v>
+                    <c:v>0.0217333905579399</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0812538848920863</c:v>
+                    <c:v>0.0740938848920863</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.18126</c:v>
+                    <c:v>0.172844158415842</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -9042,7 +9106,7 @@
                   <c:v>0.820143884892086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85</c:v>
+                  <c:v>0.841584158415842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9057,11 +9121,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130637784"/>
-        <c:axId val="-2130640888"/>
+        <c:axId val="2102589976"/>
+        <c:axId val="2102593016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130637784"/>
+        <c:axId val="2102589976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9084,7 +9148,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130640888"/>
+        <c:crossAx val="2102593016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9092,7 +9156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130640888"/>
+        <c:axId val="2102593016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -9116,7 +9180,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130637784"/>
+        <c:crossAx val="2102589976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -9124,6 +9188,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -15369,8 +15434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X486"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G40" sqref="G40:G53"/>
     </sheetView>
   </sheetViews>
@@ -16503,7 +16568,7 @@
       </c>
     </row>
     <row r="40" spans="1:24" s="143" customFormat="1" ht="37" customHeight="1">
-      <c r="B40" s="318">
+      <c r="B40" s="313">
         <v>24715505</v>
       </c>
       <c r="C40" s="163" t="s">
@@ -16534,8 +16599,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:24" s="143" customFormat="1" ht="24">
-      <c r="B41" s="318">
+    <row r="41" spans="1:24" s="143" customFormat="1" ht="48">
+      <c r="B41" s="313">
         <v>24737644</v>
       </c>
       <c r="C41" s="163" t="s">
@@ -16564,14 +16629,14 @@
       </c>
       <c r="K41" s="155"/>
     </row>
-    <row r="42" spans="1:24" s="143" customFormat="1" ht="48">
-      <c r="B42" s="318">
+    <row r="42" spans="1:24" s="143" customFormat="1" ht="36">
+      <c r="B42" s="313">
         <v>24737644</v>
       </c>
       <c r="C42" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="320" t="s">
+      <c r="D42" s="315" t="s">
         <v>1539</v>
       </c>
       <c r="E42" s="61" t="s">
@@ -16596,17 +16661,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="43" spans="1:24" s="143" customFormat="1" ht="48">
       <c r="A43" s="283" t="s">
         <v>1505</v>
       </c>
-      <c r="B43" s="319">
+      <c r="B43" s="314">
         <v>24984694</v>
       </c>
       <c r="C43" s="285" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="321" t="s">
+      <c r="D43" s="316" t="s">
         <v>694</v>
       </c>
       <c r="E43" s="284" t="s">
@@ -16645,7 +16710,7 @@
       <c r="X43" s="283"/>
     </row>
     <row r="44" spans="1:24" s="143" customFormat="1" ht="52" customHeight="1">
-      <c r="B44" s="318">
+      <c r="B44" s="313">
         <v>24984694</v>
       </c>
       <c r="C44" s="163" t="s">
@@ -16676,7 +16741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:24" s="143" customFormat="1" ht="48">
+    <row r="45" spans="1:24" s="143" customFormat="1" ht="26">
       <c r="B45" s="62">
         <v>25043933</v>
       </c>
@@ -16708,8 +16773,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:24" s="143" customFormat="1" ht="36">
-      <c r="B46" s="318">
+    <row r="46" spans="1:24" s="143" customFormat="1" ht="48">
+      <c r="B46" s="313">
         <v>24687876</v>
       </c>
       <c r="C46" s="163" t="s">
@@ -16740,8 +16805,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:24" s="143" customFormat="1" ht="48">
-      <c r="B47" s="318">
+    <row r="47" spans="1:24" s="143" customFormat="1" ht="36">
+      <c r="B47" s="313">
         <v>24687876</v>
       </c>
       <c r="C47" s="163" t="s">
@@ -16773,7 +16838,7 @@
       </c>
     </row>
     <row r="48" spans="1:24" s="143" customFormat="1" ht="36">
-      <c r="B48" s="318">
+      <c r="B48" s="313">
         <v>24687876</v>
       </c>
       <c r="C48" s="163" t="s">
@@ -16804,8 +16869,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:24" s="143" customFormat="1" ht="36">
-      <c r="B49" s="318">
+    <row r="49" spans="1:24" s="143" customFormat="1" ht="24">
+      <c r="B49" s="313">
         <v>24687876</v>
       </c>
       <c r="C49" s="163" t="s">
@@ -16836,11 +16901,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="50" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="A50" s="283" t="s">
         <v>1505</v>
       </c>
-      <c r="B50" s="319">
+      <c r="B50" s="314">
         <v>24899721</v>
       </c>
       <c r="C50" s="285" t="s">
@@ -16916,7 +16981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="52" spans="1:24" s="143" customFormat="1" ht="26">
       <c r="B52" s="61">
         <v>24954002</v>
       </c>
@@ -16948,7 +17013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="53" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B53" s="61">
         <v>25044230</v>
       </c>
@@ -16980,7 +17045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="54" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B54" s="61">
         <v>24665018</v>
       </c>
@@ -17012,8 +17077,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:24" s="143" customFormat="1" ht="24">
-      <c r="A55" s="311" t="s">
+    <row r="55" spans="1:24" s="143" customFormat="1" ht="60">
+      <c r="A55" s="306" t="s">
         <v>1540</v>
       </c>
       <c r="B55" s="61">
@@ -17047,7 +17112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="56" spans="1:24" s="143" customFormat="1" ht="33">
       <c r="B56" s="61">
         <v>24671998</v>
       </c>
@@ -17079,7 +17144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="57" spans="1:24" s="143" customFormat="1" ht="33">
       <c r="B57" s="61">
         <v>24671998</v>
       </c>
@@ -17175,7 +17240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:24" s="143" customFormat="1" ht="22">
+    <row r="60" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B60" s="61">
         <v>24687876</v>
       </c>
@@ -17207,7 +17272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:24" s="143" customFormat="1" ht="22">
+    <row r="61" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B61" s="61">
         <v>24687876</v>
       </c>
@@ -17239,7 +17304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:24" s="143" customFormat="1" ht="33">
+    <row r="62" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B62" s="61">
         <v>24715479</v>
       </c>
@@ -17269,7 +17334,7 @@
       </c>
       <c r="K62" s="155"/>
     </row>
-    <row r="63" spans="1:24" s="143" customFormat="1" ht="22">
+    <row r="63" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B63" s="61">
         <v>24715479</v>
       </c>
@@ -17301,7 +17366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:24" s="143" customFormat="1" ht="22">
+    <row r="64" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B64" s="61">
         <v>24715479</v>
       </c>
@@ -17397,7 +17462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="2:11" s="143" customFormat="1" ht="22">
+    <row r="67" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B67" s="61">
         <v>24715505</v>
       </c>
@@ -17429,7 +17494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:11" s="143" customFormat="1" ht="22">
+    <row r="68" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B68" s="61">
         <v>24715505</v>
       </c>
@@ -17461,7 +17526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="2:11" s="143" customFormat="1">
+    <row r="69" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B69" s="61">
         <v>24715505</v>
       </c>
@@ -17493,7 +17558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="2:11" s="143" customFormat="1">
+    <row r="70" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B70" s="61">
         <v>24715505</v>
       </c>
@@ -17525,7 +17590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="2:11" s="143" customFormat="1">
+    <row r="71" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B71" s="61">
         <v>24715505</v>
       </c>
@@ -17557,7 +17622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:11" s="143" customFormat="1">
+    <row r="72" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B72" s="61">
         <v>24715505</v>
       </c>
@@ -17589,7 +17654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="2:11" s="143" customFormat="1">
+    <row r="73" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B73" s="61">
         <v>24715505</v>
       </c>
@@ -17621,7 +17686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="74" spans="2:11" s="143" customFormat="1" ht="22">
       <c r="B74" s="61">
         <v>24715528</v>
       </c>
@@ -17653,7 +17718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="75" spans="2:11" s="143" customFormat="1" ht="22">
       <c r="B75" s="61">
         <v>24715528</v>
       </c>
@@ -17685,7 +17750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="2:11" s="143" customFormat="1">
+    <row r="76" spans="2:11" s="143" customFormat="1" ht="33">
       <c r="B76" s="61">
         <v>24715528</v>
       </c>
@@ -17717,14 +17782,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="2:11" s="143" customFormat="1">
+    <row r="77" spans="2:11" s="143" customFormat="1" ht="22">
       <c r="B77" s="61">
         <v>24715528</v>
       </c>
       <c r="C77" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D77" s="312" t="s">
+      <c r="D77" s="307" t="s">
         <v>1530</v>
       </c>
       <c r="E77" s="61" t="s">
@@ -17749,14 +17814,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:11" s="143" customFormat="1">
+    <row r="78" spans="2:11" s="143" customFormat="1" ht="22">
       <c r="B78" s="61">
         <v>24715528</v>
       </c>
       <c r="C78" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D78" s="312" t="s">
+      <c r="D78" s="307" t="s">
         <v>1531</v>
       </c>
       <c r="E78" s="61" t="s">
@@ -17781,7 +17846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="2:11" s="143" customFormat="1">
+    <row r="79" spans="2:11" s="143" customFormat="1" ht="22">
       <c r="B79" s="61">
         <v>24715528</v>
       </c>
@@ -17813,7 +17878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:11" s="143" customFormat="1" ht="39">
+    <row r="80" spans="2:11" s="143" customFormat="1" ht="22">
       <c r="B80" s="61">
         <v>24715528</v>
       </c>
@@ -17845,7 +17910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="81" spans="1:24" s="143" customFormat="1" ht="22">
       <c r="B81" s="61">
         <v>24715528</v>
       </c>
@@ -17877,7 +17942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:24" s="143" customFormat="1">
+    <row r="82" spans="1:24" s="143" customFormat="1" ht="22">
       <c r="B82" s="61">
         <v>24715528</v>
       </c>
@@ -17909,7 +17974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="83" spans="1:24" s="143" customFormat="1">
       <c r="B83" s="61">
         <v>24715575</v>
       </c>
@@ -17941,7 +18006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="84" spans="1:24" s="143" customFormat="1">
       <c r="B84" s="61">
         <v>24715575</v>
       </c>
@@ -18005,7 +18070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="86" spans="1:24" s="143" customFormat="1">
       <c r="B86" s="61">
         <v>24715575</v>
       </c>
@@ -18037,7 +18102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="87" spans="1:24" s="143" customFormat="1">
       <c r="B87" s="61">
         <v>24715575</v>
       </c>
@@ -18069,7 +18134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="88" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B88" s="61">
         <v>24737624</v>
       </c>
@@ -18133,7 +18198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="90" spans="1:24" s="143" customFormat="1">
       <c r="B90" s="61">
         <v>24737644</v>
       </c>
@@ -18165,7 +18230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="91" spans="1:24" s="143" customFormat="1">
       <c r="B91" s="61">
         <v>24737644</v>
       </c>
@@ -18197,8 +18262,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:24" s="143" customFormat="1">
-      <c r="A92" s="311" t="s">
+    <row r="92" spans="1:24" s="143" customFormat="1" ht="39">
+      <c r="A92" s="306" t="s">
         <v>1498</v>
       </c>
       <c r="B92" s="284">
@@ -18245,7 +18310,7 @@
       <c r="W92" s="283"/>
       <c r="X92" s="283"/>
     </row>
-    <row r="93" spans="1:24" s="143" customFormat="1">
+    <row r="93" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B93" s="61">
         <v>24740429</v>
       </c>
@@ -18309,7 +18374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:24" s="143" customFormat="1">
+    <row r="95" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B95" s="61">
         <v>24752570</v>
       </c>
@@ -18341,7 +18406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:24" s="143" customFormat="1">
+    <row r="96" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B96" s="61">
         <v>24752570</v>
       </c>
@@ -18373,7 +18438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="97" spans="2:11" s="143" customFormat="1">
       <c r="B97" s="61">
         <v>24752570</v>
       </c>
@@ -18469,7 +18534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="100" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B100" s="61">
         <v>24752666</v>
       </c>
@@ -18597,7 +18662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="2:11" s="143" customFormat="1" ht="44">
+    <row r="104" spans="2:11" s="143" customFormat="1">
       <c r="B104" s="61">
         <v>24752702</v>
       </c>
@@ -18629,7 +18694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="105" spans="2:11" s="143" customFormat="1">
       <c r="B105" s="61">
         <v>24752702</v>
       </c>
@@ -18661,7 +18726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="106" spans="2:11" s="143" customFormat="1">
       <c r="B106" s="61">
         <v>24752702</v>
       </c>
@@ -18693,7 +18758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="107" spans="2:11" s="143" customFormat="1">
       <c r="B107" s="61">
         <v>24752702</v>
       </c>
@@ -18725,7 +18790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="108" spans="2:11" s="143" customFormat="1">
       <c r="B108" s="188">
         <v>24752702</v>
       </c>
@@ -18789,7 +18854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="110" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B110" s="61">
         <v>24760871</v>
       </c>
@@ -18821,7 +18886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="143" customFormat="1" ht="60">
+    <row r="111" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B111" s="61">
         <v>24760871</v>
       </c>
@@ -18853,7 +18918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="2:11" s="143" customFormat="1" ht="60">
+    <row r="112" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B112" s="61">
         <v>24760871</v>
       </c>
@@ -18917,7 +18982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:24" s="143" customFormat="1" ht="72">
+    <row r="114" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B114" s="61">
         <v>24760871</v>
       </c>
@@ -18995,7 +19060,7 @@
       <c r="W115" s="143"/>
       <c r="X115" s="143"/>
     </row>
-    <row r="116" spans="1:24" s="143" customFormat="1" ht="65">
+    <row r="116" spans="1:24" s="143" customFormat="1" ht="44">
       <c r="B116" s="61">
         <v>24760871</v>
       </c>
@@ -19123,7 +19188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="120" spans="1:24" s="143" customFormat="1" ht="48">
       <c r="B120" s="61">
         <v>24771457</v>
       </c>
@@ -19155,7 +19220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="121" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B121" s="61">
         <v>24771457</v>
       </c>
@@ -19219,7 +19284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="123" spans="1:24" s="143" customFormat="1" ht="60">
       <c r="B123" s="61">
         <v>24782245</v>
       </c>
@@ -19249,7 +19314,7 @@
       </c>
       <c r="K123" s="155"/>
     </row>
-    <row r="124" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="124" spans="1:24" s="143" customFormat="1" ht="60">
       <c r="B124" s="61">
         <v>24782245</v>
       </c>
@@ -19281,7 +19346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:24" s="143" customFormat="1">
+    <row r="125" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B125" s="61">
         <v>24782245</v>
       </c>
@@ -19313,7 +19378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:24" s="143" customFormat="1">
+    <row r="126" spans="1:24" s="143" customFormat="1" ht="72">
       <c r="B126" s="61">
         <v>24782245</v>
       </c>
@@ -19345,7 +19410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:24" s="143" customFormat="1">
+    <row r="127" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B127" s="61">
         <v>24782245</v>
       </c>
@@ -19377,7 +19442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:24" s="143" customFormat="1">
+    <row r="128" spans="1:24" s="143" customFormat="1" ht="65">
       <c r="A128" s="283" t="s">
         <v>1500</v>
       </c>
@@ -19425,7 +19490,7 @@
       <c r="W128" s="283"/>
       <c r="X128" s="283"/>
     </row>
-    <row r="129" spans="2:11" s="143" customFormat="1">
+    <row r="129" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B129" s="61">
         <v>24790185</v>
       </c>
@@ -19457,7 +19522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="2:11" s="143" customFormat="1">
+    <row r="130" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B130" s="61">
         <v>24790185</v>
       </c>
@@ -19489,7 +19554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="2:11" s="143" customFormat="1">
+    <row r="131" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B131" s="61">
         <v>24790185</v>
       </c>
@@ -19521,7 +19586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="2:11" s="143" customFormat="1">
+    <row r="132" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B132" s="61">
         <v>24790185</v>
       </c>
@@ -19553,7 +19618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="143" customFormat="1">
+    <row r="133" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B133" s="61">
         <v>24790185</v>
       </c>
@@ -19585,7 +19650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="143" customFormat="1">
+    <row r="134" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B134" s="61">
         <v>24790185</v>
       </c>
@@ -19617,7 +19682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="143" customFormat="1">
+    <row r="135" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B135" s="61">
         <v>24790185</v>
       </c>
@@ -19649,7 +19714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="143" customFormat="1">
+    <row r="136" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B136" s="61">
         <v>24790185</v>
       </c>
@@ -19681,7 +19746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="137" spans="2:11" s="143" customFormat="1">
       <c r="B137" s="61">
         <v>24825750</v>
       </c>
@@ -19713,7 +19778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="138" spans="2:11" s="143" customFormat="1">
       <c r="B138" s="61">
         <v>24825750</v>
       </c>
@@ -19745,7 +19810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="139" spans="2:11" s="143" customFormat="1">
       <c r="B139" s="61">
         <v>24825750</v>
       </c>
@@ -19777,7 +19842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="140" spans="2:11" s="143" customFormat="1">
       <c r="B140" s="61">
         <v>24825750</v>
       </c>
@@ -19809,7 +19874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="141" spans="2:11" s="143" customFormat="1">
       <c r="B141" s="61">
         <v>24825750</v>
       </c>
@@ -19841,7 +19906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="142" spans="2:11" s="143" customFormat="1">
       <c r="B142" s="61">
         <v>24825750</v>
       </c>
@@ -19873,7 +19938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="143" spans="2:11" s="143" customFormat="1">
       <c r="B143" s="188">
         <v>24825750</v>
       </c>
@@ -19905,7 +19970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="144" spans="2:11" s="143" customFormat="1">
       <c r="B144" s="188">
         <v>24825750</v>
       </c>
@@ -19937,7 +20002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="145" spans="1:24" s="143" customFormat="1">
       <c r="B145" s="188">
         <v>24825750</v>
       </c>
@@ -19969,7 +20034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="146" spans="1:24" s="143" customFormat="1">
       <c r="B146" s="188">
         <v>24825750</v>
       </c>
@@ -20001,7 +20066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="147" spans="1:24" s="143" customFormat="1">
       <c r="B147" s="188">
         <v>24825750</v>
       </c>
@@ -20033,7 +20098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="148" spans="1:24" s="143" customFormat="1">
       <c r="B148" s="188">
         <v>24825750</v>
       </c>
@@ -20065,7 +20130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="149" spans="1:24" s="143" customFormat="1" ht="48">
       <c r="B149" s="188">
         <v>24825798</v>
       </c>
@@ -20095,7 +20160,7 @@
       </c>
       <c r="K149" s="155"/>
     </row>
-    <row r="150" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="150" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B150" s="188">
         <v>24849359</v>
       </c>
@@ -20159,7 +20224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:24" s="283" customFormat="1" ht="24">
+    <row r="152" spans="1:24" s="283" customFormat="1" ht="36">
       <c r="A152" s="143"/>
       <c r="B152" s="181">
         <v>24849359</v>
@@ -20205,7 +20270,7 @@
       <c r="W152" s="143"/>
       <c r="X152" s="143"/>
     </row>
-    <row r="153" spans="1:24" s="143" customFormat="1" ht="48">
+    <row r="153" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B153" s="188">
         <v>24849359</v>
       </c>
@@ -20333,7 +20398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="157" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B157" s="188">
         <v>24899700</v>
       </c>
@@ -20397,7 +20462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="159" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B159" s="61">
         <v>24899700</v>
       </c>
@@ -20461,7 +20526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="161" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B161" s="188">
         <v>24899700</v>
       </c>
@@ -20589,7 +20654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="165" spans="2:11" s="143" customFormat="1" ht="48">
       <c r="B165" s="61">
         <v>24920620</v>
       </c>
@@ -20685,7 +20750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="168" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B168" s="181">
         <v>24920620</v>
       </c>
@@ -20781,7 +20846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="171" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B171" s="181">
         <v>24920620</v>
       </c>
@@ -20845,7 +20910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="173" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B173" s="181">
         <v>24920620</v>
       </c>
@@ -20877,7 +20942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="174" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B174" s="181">
         <v>24920620</v>
       </c>
@@ -20909,7 +20974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="143" customFormat="1" ht="33">
+    <row r="175" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B175" s="181">
         <v>24920620</v>
       </c>
@@ -20941,7 +21006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="176" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B176" s="181">
         <v>24920620</v>
       </c>
@@ -20973,7 +21038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="177" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B177" s="181">
         <v>24920620</v>
       </c>
@@ -21037,7 +21102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="179" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B179" s="181">
         <v>24920620</v>
       </c>
@@ -21069,7 +21134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="180" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B180" s="181">
         <v>24920622</v>
       </c>
@@ -21101,7 +21166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="181" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B181" s="181">
         <v>24920622</v>
       </c>
@@ -21133,7 +21198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="182" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B182" s="188">
         <v>24920622</v>
       </c>
@@ -21165,7 +21230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="183" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B183" s="188">
         <v>24920622</v>
       </c>
@@ -21197,7 +21262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="2:11" s="143" customFormat="1" ht="33">
+    <row r="184" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B184" s="188">
         <v>24920622</v>
       </c>
@@ -21229,7 +21294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="2:11" s="143" customFormat="1" ht="33">
+    <row r="185" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B185" s="188">
         <v>24920622</v>
       </c>
@@ -21261,7 +21326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="186" spans="2:11" s="143" customFormat="1" ht="48">
       <c r="B186" s="188">
         <v>24920622</v>
       </c>
@@ -21293,7 +21358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="187" spans="2:11" s="143" customFormat="1" ht="33">
       <c r="B187" s="188">
         <v>24920622</v>
       </c>
@@ -21323,7 +21388,7 @@
       </c>
       <c r="K187" s="155"/>
     </row>
-    <row r="188" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="188" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B188" s="188">
         <v>24920622</v>
       </c>
@@ -21387,7 +21452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="190" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B190" s="188">
         <v>24920622</v>
       </c>
@@ -21419,7 +21484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="191" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B191" s="188">
         <v>24920622</v>
       </c>
@@ -21451,7 +21516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="192" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B192" s="188">
         <v>24920622</v>
       </c>
@@ -21483,7 +21548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="193" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B193" s="188">
         <v>24920622</v>
       </c>
@@ -21515,7 +21580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="194" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B194" s="61">
         <v>24920622</v>
       </c>
@@ -21547,7 +21612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:24" s="143" customFormat="1" ht="33">
+    <row r="195" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B195" s="61">
         <v>24920622</v>
       </c>
@@ -21579,7 +21644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="196" spans="1:24" s="143" customFormat="1" ht="33">
       <c r="B196" s="61">
         <v>24920622</v>
       </c>
@@ -21611,7 +21676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="197" spans="1:24" s="143" customFormat="1" ht="33">
       <c r="B197" s="61">
         <v>24920622</v>
       </c>
@@ -21643,7 +21708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="198" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B198" s="61">
         <v>24920622</v>
       </c>
@@ -21787,7 +21852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="202" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B202" s="61">
         <v>24942187</v>
       </c>
@@ -21883,7 +21948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:24" s="143" customFormat="1" ht="39">
+    <row r="205" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B205" s="188">
         <v>24966368</v>
       </c>
@@ -21915,7 +21980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:24" s="143" customFormat="1" ht="48">
+    <row r="206" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B206" s="188">
         <v>24966368</v>
       </c>
@@ -21947,7 +22012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:24" s="143" customFormat="1" ht="48">
+    <row r="207" spans="1:24" s="143" customFormat="1" ht="33">
       <c r="B207" s="188">
         <v>24966380</v>
       </c>
@@ -22011,7 +22076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:24" s="143" customFormat="1" ht="60">
+    <row r="209" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B209" s="188">
         <v>24966384</v>
       </c>
@@ -22043,7 +22108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:24" s="143" customFormat="1" ht="48">
+    <row r="210" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B210" s="188">
         <v>24966384</v>
       </c>
@@ -22075,7 +22140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:24" s="143" customFormat="1">
+    <row r="211" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B211" s="188">
         <v>24966384</v>
       </c>
@@ -22107,7 +22172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:24" s="143" customFormat="1">
+    <row r="212" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B212" s="188">
         <v>24966384</v>
       </c>
@@ -22139,7 +22204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:24" s="143" customFormat="1">
+    <row r="213" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B213" s="188">
         <v>24966384</v>
       </c>
@@ -22171,7 +22236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:24" s="143" customFormat="1">
+    <row r="214" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B214" s="188">
         <v>24966384</v>
       </c>
@@ -22203,7 +22268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="1:24" s="143" customFormat="1">
+    <row r="215" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B215" s="188">
         <v>24966384</v>
       </c>
@@ -22235,7 +22300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:24" s="143" customFormat="1">
+    <row r="216" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B216" s="188">
         <v>24966384</v>
       </c>
@@ -22267,7 +22332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="217" spans="1:24" s="143" customFormat="1" ht="39">
       <c r="B217" s="61">
         <v>24966384</v>
       </c>
@@ -22297,7 +22362,7 @@
       </c>
       <c r="K217" s="155"/>
     </row>
-    <row r="218" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="218" spans="1:24" s="143" customFormat="1" ht="48">
       <c r="B218" s="61">
         <v>24984694</v>
       </c>
@@ -22361,7 +22426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="220" spans="1:24" s="143" customFormat="1" ht="60">
       <c r="B220" s="61">
         <v>24984694</v>
       </c>
@@ -22391,7 +22456,7 @@
       </c>
       <c r="K220" s="161"/>
     </row>
-    <row r="221" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="221" spans="1:24" s="143" customFormat="1">
       <c r="A221" s="283" t="s">
         <v>1500</v>
       </c>
@@ -22439,7 +22504,7 @@
       <c r="W221" s="283"/>
       <c r="X221" s="283"/>
     </row>
-    <row r="222" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="222" spans="1:24" s="143" customFormat="1">
       <c r="A222" s="283" t="s">
         <v>1500</v>
       </c>
@@ -22487,7 +22552,7 @@
       <c r="W222" s="283"/>
       <c r="X222" s="283"/>
     </row>
-    <row r="223" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="223" spans="1:24" s="143" customFormat="1">
       <c r="A223" s="283" t="s">
         <v>1500</v>
       </c>
@@ -22535,7 +22600,7 @@
       <c r="W223" s="283"/>
       <c r="X223" s="283"/>
     </row>
-    <row r="224" spans="1:24" s="283" customFormat="1" ht="24">
+    <row r="224" spans="1:24" s="283" customFormat="1">
       <c r="A224" s="283" t="s">
         <v>1500</v>
       </c>
@@ -22570,7 +22635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="225" spans="1:24" s="143" customFormat="1">
       <c r="A225" s="283" t="s">
         <v>1500</v>
       </c>
@@ -22580,7 +22645,7 @@
       <c r="C225" s="263" t="s">
         <v>2</v>
       </c>
-      <c r="D225" s="315" t="s">
+      <c r="D225" s="310" t="s">
         <v>1521</v>
       </c>
       <c r="E225" s="263" t="s">
@@ -22618,7 +22683,7 @@
       <c r="W225" s="283"/>
       <c r="X225" s="283"/>
     </row>
-    <row r="226" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="226" spans="1:24" s="143" customFormat="1">
       <c r="A226" s="283" t="s">
         <v>1500</v>
       </c>
@@ -22776,7 +22841,7 @@
       <c r="W229" s="143"/>
       <c r="X229" s="143"/>
     </row>
-    <row r="230" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="230" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B230" s="62">
         <v>25009260</v>
       </c>
@@ -22872,7 +22937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="233" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B233" s="62">
         <v>25009260</v>
       </c>
@@ -22943,7 +23008,7 @@
       <c r="C235" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="D235" s="314" t="s">
+      <c r="D235" s="309" t="s">
         <v>670</v>
       </c>
       <c r="E235" s="176" t="s">
@@ -22968,7 +23033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="236" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B236" s="62">
         <v>25009260</v>
       </c>
@@ -23071,7 +23136,7 @@
       <c r="C239" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="D239" s="313" t="s">
+      <c r="D239" s="308" t="s">
         <v>673</v>
       </c>
       <c r="E239" s="176" t="s">
@@ -23096,7 +23161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="240" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B240" s="62">
         <v>25009276</v>
       </c>
@@ -23224,7 +23289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="244" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B244" s="62">
         <v>25009276</v>
       </c>
@@ -23320,7 +23385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="247" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B247" s="62">
         <v>25009276</v>
       </c>
@@ -23416,7 +23481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="250" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B250" s="61">
         <v>25031392</v>
       </c>
@@ -23544,7 +23609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="254" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="254" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B254" s="61">
         <v>25031414</v>
       </c>
@@ -23576,7 +23641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="255" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B255" s="61">
         <v>25031414</v>
       </c>
@@ -23608,7 +23673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="256" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B256" s="61">
         <v>25031414</v>
       </c>
@@ -23640,7 +23705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="257" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B257" s="61">
         <v>25031414</v>
       </c>
@@ -23672,7 +23737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="258" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B258" s="61">
         <v>25031414</v>
       </c>
@@ -23704,7 +23769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="259" spans="2:11" s="143" customFormat="1" ht="39">
+    <row r="259" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B259" s="61">
         <v>25031414</v>
       </c>
@@ -23736,7 +23801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="260" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B260" s="61">
         <v>25031414</v>
       </c>
@@ -23768,7 +23833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="261" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B261" s="61">
         <v>25031414</v>
       </c>
@@ -23800,7 +23865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="262" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B262" s="61">
         <v>25031414</v>
       </c>
@@ -23832,7 +23897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="263" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B263" s="61">
         <v>25031414</v>
       </c>
@@ -23864,7 +23929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="264" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B264" s="62">
         <v>25043553</v>
       </c>
@@ -23928,7 +23993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="266" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B266" s="62">
         <v>25043933</v>
       </c>
@@ -23960,7 +24025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="267" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B267" s="62">
         <v>25043933</v>
       </c>
@@ -23992,7 +24057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="268" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B268" s="62">
         <v>25043933</v>
       </c>
@@ -24024,7 +24089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="269" spans="2:11" s="143" customFormat="1" ht="39">
       <c r="B269" s="62">
         <v>25043933</v>
       </c>
@@ -24056,7 +24121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="270" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B270" s="62">
         <v>25043933</v>
       </c>
@@ -24088,7 +24153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="271" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B271" s="62">
         <v>25043933</v>
       </c>
@@ -24120,7 +24185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="272" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B272" s="62">
         <v>25043933</v>
       </c>
@@ -24152,7 +24217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="273" spans="1:24" s="143" customFormat="1" ht="26">
       <c r="B273" s="62">
         <v>25043933</v>
       </c>
@@ -24184,7 +24249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="274" spans="1:24" s="143" customFormat="1" ht="26">
       <c r="B274" s="62">
         <v>25043933</v>
       </c>
@@ -24216,7 +24281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="275" spans="1:24" s="143" customFormat="1" ht="48">
       <c r="B275" s="61">
         <v>25044160</v>
       </c>
@@ -24248,7 +24313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="276" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B276" s="61">
         <v>25044160</v>
       </c>
@@ -24280,7 +24345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="277" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B277" s="61">
         <v>25044160</v>
       </c>
@@ -24312,7 +24377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="278" spans="1:24" s="143" customFormat="1" ht="48">
       <c r="B278" s="61">
         <v>25044160</v>
       </c>
@@ -24390,7 +24455,7 @@
       <c r="W279" s="143"/>
       <c r="X279" s="143"/>
     </row>
-    <row r="280" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="280" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B280" s="61">
         <v>25080583</v>
       </c>
@@ -24422,7 +24487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="281" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B281" s="61">
         <v>25080583</v>
       </c>
@@ -24454,7 +24519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="282" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B282" s="61">
         <v>25100594</v>
       </c>
@@ -24518,7 +24583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="284" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B284" s="61">
         <v>25100594</v>
       </c>
@@ -24774,7 +24839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="292" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="292" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B292" s="61">
         <v>25100594</v>
       </c>
@@ -24998,7 +25063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="299" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="299" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B299" s="188">
         <v>25100604</v>
       </c>
@@ -25030,7 +25095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="300" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="300" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B300" s="188">
         <v>25100604</v>
       </c>
@@ -25222,7 +25287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="306" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B306" s="188">
         <v>25100604</v>
       </c>
@@ -25318,7 +25383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="309" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="309" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B309" s="218">
         <v>25177484</v>
       </c>
@@ -25350,7 +25415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="310" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B310" s="218">
         <v>25177484</v>
       </c>
@@ -25382,7 +25447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="311" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="311" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B311" s="218">
         <v>25177484</v>
       </c>
@@ -25414,7 +25479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="312" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="312" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B312" s="218">
         <v>25177484</v>
       </c>
@@ -25446,7 +25511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="313" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="313" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B313" s="218">
         <v>25177484</v>
       </c>
@@ -25478,7 +25543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="314" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="314" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B314" s="218">
         <v>25177484</v>
       </c>
@@ -25542,7 +25607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="316" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="316" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B316" s="218">
         <v>25177484</v>
       </c>
@@ -25574,7 +25639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="317" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B317" s="218">
         <v>25177484</v>
       </c>
@@ -25638,7 +25703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="319" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="319" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B319" s="218">
         <v>25202271</v>
       </c>
@@ -25670,7 +25735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="320" spans="2:11" s="143" customFormat="1" ht="48">
       <c r="B320" s="218">
         <v>25202271</v>
       </c>
@@ -25702,7 +25767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="321" spans="1:24" s="283" customFormat="1" ht="24">
+    <row r="321" spans="1:24" s="283" customFormat="1" ht="36">
       <c r="A321" s="143"/>
       <c r="B321" s="218">
         <v>25202271</v>
@@ -25748,7 +25813,7 @@
       <c r="W321" s="143"/>
       <c r="X321" s="143"/>
     </row>
-    <row r="322" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="322" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B322" s="218">
         <v>25202271</v>
       </c>
@@ -25780,7 +25845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="323" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="323" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B323" s="218">
         <v>25202271</v>
       </c>
@@ -25812,7 +25877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="324" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="324" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B324" s="218">
         <v>25202271</v>
       </c>
@@ -25844,7 +25909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="325" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B325" s="218">
         <v>25202271</v>
       </c>
@@ -26114,7 +26179,7 @@
       <c r="W332" s="143"/>
       <c r="X332" s="143"/>
     </row>
-    <row r="333" spans="1:24" s="283" customFormat="1" ht="13">
+    <row r="333" spans="1:24" s="283" customFormat="1" ht="24">
       <c r="A333" s="143"/>
       <c r="B333" s="181">
         <v>24659141</v>
@@ -26206,7 +26271,7 @@
       <c r="W334" s="143"/>
       <c r="X334" s="143"/>
     </row>
-    <row r="335" spans="1:24" s="283" customFormat="1">
+    <row r="335" spans="1:24" s="283" customFormat="1" ht="24">
       <c r="A335" s="143"/>
       <c r="B335" s="181">
         <v>24659141</v>
@@ -26252,7 +26317,7 @@
       <c r="W335" s="143"/>
       <c r="X335" s="143"/>
     </row>
-    <row r="336" spans="1:24" s="283" customFormat="1">
+    <row r="336" spans="1:24" s="283" customFormat="1" ht="24">
       <c r="A336" s="143"/>
       <c r="B336" s="181">
         <v>24659141</v>
@@ -26298,7 +26363,7 @@
       <c r="W336" s="143"/>
       <c r="X336" s="143"/>
     </row>
-    <row r="337" spans="1:24" s="283" customFormat="1">
+    <row r="337" spans="1:24" s="283" customFormat="1" ht="24">
       <c r="A337" s="143"/>
       <c r="B337" s="181">
         <v>24659141</v>
@@ -26344,7 +26409,7 @@
       <c r="W337" s="143"/>
       <c r="X337" s="143"/>
     </row>
-    <row r="338" spans="1:24" s="143" customFormat="1">
+    <row r="338" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B338" s="188">
         <v>24659141</v>
       </c>
@@ -26376,7 +26441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:24" s="143" customFormat="1">
+    <row r="339" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B339" s="188">
         <v>24659141</v>
       </c>
@@ -26408,7 +26473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="340" spans="1:24" s="143" customFormat="1">
+    <row r="340" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B340" s="188">
         <v>24659141</v>
       </c>
@@ -26440,7 +26505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:24" s="143" customFormat="1">
+    <row r="341" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B341" s="188">
         <v>24659141</v>
       </c>
@@ -26472,14 +26537,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:24" s="143" customFormat="1">
+    <row r="342" spans="1:24" s="143" customFormat="1" ht="13">
       <c r="B342" s="188">
         <v>24659141</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="D342" s="317" t="s">
+      <c r="D342" s="312" t="s">
         <v>1404</v>
       </c>
       <c r="E342" s="157" t="s">
@@ -26504,7 +26569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:24" s="143" customFormat="1">
+    <row r="343" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B343" s="188">
         <v>24659141</v>
       </c>
@@ -26543,7 +26608,7 @@
       <c r="C344" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="D344" s="312" t="s">
+      <c r="D344" s="307" t="s">
         <v>925</v>
       </c>
       <c r="E344" s="61" t="s">
@@ -26575,7 +26640,7 @@
       <c r="C345" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="D345" s="312" t="s">
+      <c r="D345" s="307" t="s">
         <v>926</v>
       </c>
       <c r="E345" s="61" t="s">
@@ -26607,7 +26672,7 @@
       <c r="C346" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="D346" s="312" t="s">
+      <c r="D346" s="307" t="s">
         <v>912</v>
       </c>
       <c r="E346" s="61" t="s">
@@ -26632,7 +26697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="347" spans="1:24" s="143" customFormat="1" ht="48">
+    <row r="347" spans="1:24" s="143" customFormat="1">
       <c r="B347" s="61">
         <v>24668417</v>
       </c>
@@ -26664,14 +26729,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="348" spans="1:24" s="143" customFormat="1">
       <c r="B348" s="61">
         <v>24668417</v>
       </c>
       <c r="C348" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D348" s="312" t="s">
+      <c r="D348" s="307" t="s">
         <v>914</v>
       </c>
       <c r="E348" s="61" t="s">
@@ -26696,7 +26761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="349" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="349" spans="1:24" s="143" customFormat="1">
       <c r="B349" s="61">
         <v>24668417</v>
       </c>
@@ -26728,7 +26793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="350" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="350" spans="1:24" s="143" customFormat="1">
       <c r="B350" s="61">
         <v>24668417</v>
       </c>
@@ -26760,7 +26825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="351" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="351" spans="1:24" s="143" customFormat="1">
       <c r="B351" s="61">
         <v>24668417</v>
       </c>
@@ -26792,7 +26857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="352" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="352" spans="1:24" s="143" customFormat="1">
       <c r="B352" s="61">
         <v>24668417</v>
       </c>
@@ -26824,7 +26889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="353" spans="1:11" s="143" customFormat="1" ht="24">
+    <row r="353" spans="1:11" s="143" customFormat="1">
       <c r="B353" s="61">
         <v>24668417</v>
       </c>
@@ -26856,7 +26921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:11" s="143" customFormat="1" ht="36">
+    <row r="354" spans="1:11" s="143" customFormat="1">
       <c r="B354" s="61">
         <v>24668417</v>
       </c>
@@ -26888,7 +26953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="355" spans="1:11" s="143" customFormat="1" ht="24">
+    <row r="355" spans="1:11" s="143" customFormat="1">
       <c r="B355" s="61">
         <v>24668417</v>
       </c>
@@ -26952,7 +27017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="357" spans="1:11" s="143" customFormat="1" ht="60">
+    <row r="357" spans="1:11" s="143" customFormat="1" ht="36">
       <c r="B357" s="61">
         <v>24825607</v>
       </c>
@@ -26984,14 +27049,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:11" s="143" customFormat="1" ht="36">
+    <row r="358" spans="1:11" s="143" customFormat="1" ht="24">
       <c r="B358" s="188">
         <v>24825838</v>
       </c>
       <c r="C358" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D358" s="308" t="s">
+      <c r="D358" s="303" t="s">
         <v>1503</v>
       </c>
       <c r="E358" s="61" t="s">
@@ -27023,7 +27088,7 @@
       <c r="C359" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D359" s="309" t="s">
+      <c r="D359" s="304" t="s">
         <v>1501</v>
       </c>
       <c r="E359" s="61" t="s">
@@ -27055,7 +27120,7 @@
       <c r="C360" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D360" s="309" t="s">
+      <c r="D360" s="304" t="s">
         <v>1502</v>
       </c>
       <c r="E360" s="61" t="s">
@@ -27080,7 +27145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="1:11" s="143" customFormat="1" ht="24">
+    <row r="361" spans="1:11" s="143" customFormat="1" ht="36">
       <c r="B361" s="188">
         <v>24849359</v>
       </c>
@@ -27112,7 +27177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="362" spans="1:11" s="143" customFormat="1" ht="24">
+    <row r="362" spans="1:11" s="143" customFormat="1" ht="60">
       <c r="B362" s="188">
         <v>24855015</v>
       </c>
@@ -27142,7 +27207,7 @@
       </c>
       <c r="K362" s="155"/>
     </row>
-    <row r="363" spans="1:11" s="143" customFormat="1" ht="24">
+    <row r="363" spans="1:11" s="143" customFormat="1" ht="36">
       <c r="B363" s="188">
         <v>24855015</v>
       </c>
@@ -27174,7 +27239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="364" spans="1:11" s="143" customFormat="1" ht="24">
+    <row r="364" spans="1:11" s="143" customFormat="1" ht="36">
       <c r="B364" s="188">
         <v>24899700</v>
       </c>
@@ -27868,7 +27933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="384" spans="1:11" s="143" customFormat="1" ht="60">
+    <row r="384" spans="1:11" s="143" customFormat="1" ht="24">
       <c r="A384" s="143" t="s">
         <v>1536</v>
       </c>
@@ -27903,7 +27968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="385" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="385" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="A385" s="143" t="s">
         <v>1536</v>
       </c>
@@ -28008,7 +28073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="388" spans="1:24" s="143" customFormat="1" ht="36">
+    <row r="388" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="A388" s="143" t="s">
         <v>1536</v>
       </c>
@@ -28139,7 +28204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="392" spans="1:24" s="143" customFormat="1" ht="13">
+    <row r="392" spans="1:24" s="143" customFormat="1" ht="36">
       <c r="B392" s="61">
         <v>24899721</v>
       </c>
@@ -28171,7 +28236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="1:24" s="143" customFormat="1" ht="13">
+    <row r="393" spans="1:24" s="143" customFormat="1" ht="24">
       <c r="B393" s="61">
         <v>24906209</v>
       </c>
@@ -28235,7 +28300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="395" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="395" spans="1:24" s="143" customFormat="1" ht="13">
       <c r="B395" s="61">
         <v>24906209</v>
       </c>
@@ -28267,7 +28332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="396" spans="1:24" s="143" customFormat="1" ht="24">
+    <row r="396" spans="1:24" s="143" customFormat="1" ht="13">
       <c r="A396" s="283" t="s">
         <v>1500</v>
       </c>
@@ -28277,7 +28342,7 @@
       <c r="C396" s="285" t="s">
         <v>61</v>
       </c>
-      <c r="D396" s="316" t="s">
+      <c r="D396" s="311" t="s">
         <v>1506</v>
       </c>
       <c r="E396" s="286" t="s">
@@ -28443,7 +28508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="401" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B401" s="61">
         <v>24920616</v>
       </c>
@@ -28475,7 +28540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="402" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B402" s="61">
         <v>24920619</v>
       </c>
@@ -28507,7 +28572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="403" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="403" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B403" s="61">
         <v>24920619</v>
       </c>
@@ -28539,7 +28604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="404" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="404" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B404" s="61">
         <v>24920619</v>
       </c>
@@ -28571,7 +28636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="405" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="405" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B405" s="61">
         <v>24920619</v>
       </c>
@@ -28603,7 +28668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="406" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="406" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B406" s="61">
         <v>24920619</v>
       </c>
@@ -28667,7 +28732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="408" spans="2:11" s="143" customFormat="1">
+    <row r="408" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B408" s="61">
         <v>24920621</v>
       </c>
@@ -28699,7 +28764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="409" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="409" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B409" s="61">
         <v>24954002</v>
       </c>
@@ -28731,7 +28796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="410" spans="2:11" s="143" customFormat="1" ht="26">
+    <row r="410" spans="2:11" s="143" customFormat="1">
       <c r="B410" s="61">
         <v>24954002</v>
       </c>
@@ -28795,7 +28860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="412" spans="2:11" s="143" customFormat="1" ht="39">
+    <row r="412" spans="2:11" s="143" customFormat="1" ht="26">
       <c r="B412" s="61">
         <v>24954002</v>
       </c>
@@ -28827,7 +28892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="413" spans="2:11" s="143" customFormat="1">
+    <row r="413" spans="2:11" s="143" customFormat="1" ht="39">
       <c r="B413" s="61">
         <v>24954002</v>
       </c>
@@ -28859,7 +28924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="414" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="414" spans="2:11" s="143" customFormat="1">
       <c r="B414" s="61">
         <v>24954002</v>
       </c>
@@ -28891,7 +28956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="415" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="415" spans="2:11" s="143" customFormat="1" ht="48">
       <c r="B415" s="61">
         <v>24956542</v>
       </c>
@@ -28923,7 +28988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="416" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="416" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B416" s="61">
         <v>24956542</v>
       </c>
@@ -28987,7 +29052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="418" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="418" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B418" s="61">
         <v>24956542</v>
       </c>
@@ -29147,7 +29212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="423" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="423" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B423" s="61">
         <v>24956542</v>
       </c>
@@ -29179,7 +29244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="424" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="424" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B424" s="61">
         <v>24956542</v>
       </c>
@@ -29275,7 +29340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="427" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="427" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B427" s="61">
         <v>24956542</v>
       </c>
@@ -29339,7 +29404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="429" spans="2:11" s="143" customFormat="1" ht="48">
+    <row r="429" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B429" s="61">
         <v>24956542</v>
       </c>
@@ -29371,7 +29436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="430" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="430" spans="2:11" s="143" customFormat="1" ht="48">
       <c r="B430" s="61">
         <v>24956542</v>
       </c>
@@ -29403,7 +29468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="431" spans="2:11" s="143" customFormat="1" ht="13">
+    <row r="431" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B431" s="61">
         <v>24966369</v>
       </c>
@@ -29499,7 +29564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="434" spans="2:11" s="143" customFormat="1" ht="52">
+    <row r="434" spans="2:11" s="143" customFormat="1" ht="13">
       <c r="B434" s="297">
         <v>24990918</v>
       </c>
@@ -29531,7 +29596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="435" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="435" spans="2:11" s="143" customFormat="1" ht="52">
       <c r="B435" s="297">
         <v>24990918</v>
       </c>
@@ -29563,7 +29628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="436" spans="2:11" s="143" customFormat="1" ht="24">
+    <row r="436" spans="2:11" s="143" customFormat="1" ht="36">
       <c r="B436" s="297">
         <v>24990918</v>
       </c>
@@ -29723,7 +29788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="441" spans="2:11" s="143" customFormat="1" ht="36">
+    <row r="441" spans="2:11" s="143" customFormat="1" ht="24">
       <c r="B441" s="62">
         <v>25043676</v>
       </c>
@@ -30616,7 +30681,7 @@
       <c r="C469" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="D469" s="310" t="s">
+      <c r="D469" s="305" t="s">
         <v>1526</v>
       </c>
       <c r="E469" s="157" t="s">
@@ -32848,8 +32913,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="G95" sqref="G95"/>
     </sheetView>
@@ -34798,7 +34863,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="24">
+    <row r="87" spans="1:11" ht="12">
       <c r="B87" s="15">
         <v>24760871</v>
       </c>
@@ -34850,7 +34915,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="22">
+    <row r="89" spans="1:11" ht="84">
       <c r="A89" s="259" t="s">
         <v>1483</v>
       </c>
@@ -34860,7 +34925,7 @@
       <c r="C89" s="261" t="s">
         <v>271</v>
       </c>
-      <c r="D89" s="326" t="s">
+      <c r="D89" s="321" t="s">
         <v>1443</v>
       </c>
       <c r="E89" s="256" t="s">
@@ -34933,7 +34998,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="12">
+    <row r="92" spans="1:11" ht="24">
       <c r="A92" s="255" t="s">
         <v>1484</v>
       </c>
@@ -34964,7 +35029,7 @@
       <c r="J92" s="255"/>
       <c r="K92" s="255"/>
     </row>
-    <row r="93" spans="1:11" ht="36">
+    <row r="93" spans="1:11" ht="26">
       <c r="B93" s="10">
         <v>25031397</v>
       </c>
@@ -34990,7 +35055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="12">
+    <row r="94" spans="1:11" ht="39">
       <c r="B94" s="15">
         <v>25099614</v>
       </c>
@@ -35018,7 +35083,7 @@
       <c r="J94" s="230"/>
       <c r="K94" s="12"/>
     </row>
-    <row r="95" spans="1:11" ht="24">
+    <row r="95" spans="1:11" ht="36">
       <c r="A95" s="259" t="s">
         <v>1488</v>
       </c>
@@ -35028,7 +35093,7 @@
       <c r="C95" s="256" t="s">
         <v>412</v>
       </c>
-      <c r="D95" s="325" t="s">
+      <c r="D95" s="320" t="s">
         <v>413</v>
       </c>
       <c r="E95" s="258" t="s">
@@ -35049,7 +35114,7 @@
       <c r="J95" s="255"/>
       <c r="K95" s="255"/>
     </row>
-    <row r="96" spans="1:11" ht="24">
+    <row r="96" spans="1:11" ht="36">
       <c r="B96" s="15">
         <v>24668417</v>
       </c>
@@ -35077,7 +35142,7 @@
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="2:9" ht="12">
+    <row r="97" spans="2:9" ht="22">
       <c r="B97" s="15">
         <v>24671998</v>
       </c>
@@ -35103,7 +35168,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="98" spans="2:9" ht="12">
+    <row r="98" spans="2:9" ht="36">
       <c r="B98" s="15">
         <v>24687876</v>
       </c>
@@ -35129,7 +35194,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="99" spans="2:9" ht="24">
+    <row r="99" spans="2:9" ht="12">
       <c r="B99" s="15">
         <v>24687876</v>
       </c>
@@ -35155,7 +35220,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="100" spans="2:9" ht="24">
+    <row r="100" spans="2:9" ht="12">
       <c r="B100" s="15">
         <v>24687876</v>
       </c>
@@ -35181,7 +35246,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="101" spans="2:9" ht="13">
+    <row r="101" spans="2:9" ht="36">
       <c r="B101" s="15">
         <v>24737624</v>
       </c>
@@ -35285,7 +35350,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="105" spans="2:9" ht="22">
+    <row r="105" spans="2:9" ht="12">
       <c r="B105" s="15">
         <v>24752666</v>
       </c>
@@ -35337,7 +35402,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="107" spans="2:9" ht="12">
+    <row r="107" spans="2:9" ht="24">
       <c r="B107" s="15">
         <v>24752702</v>
       </c>
@@ -35363,7 +35428,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="108" spans="2:9" ht="60">
+    <row r="108" spans="2:9" ht="24">
       <c r="B108" s="15">
         <v>24752702</v>
       </c>
@@ -35389,7 +35454,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="109" spans="2:9" ht="24">
+    <row r="109" spans="2:9" ht="22">
       <c r="B109" s="15">
         <v>24790185</v>
       </c>
@@ -35415,7 +35480,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="110" spans="2:9" ht="24">
+    <row r="110" spans="2:9" ht="12">
       <c r="B110" s="15">
         <v>24825750</v>
       </c>
@@ -35441,7 +35506,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="111" spans="2:9" ht="24">
+    <row r="111" spans="2:9" ht="12">
       <c r="B111" s="15">
         <v>24825750</v>
       </c>
@@ -35467,7 +35532,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="112" spans="2:9" ht="24">
+    <row r="112" spans="2:9" ht="60">
       <c r="B112" s="15">
         <v>24825838</v>
       </c>
@@ -35493,7 +35558,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="113" spans="1:11" s="255" customFormat="1" ht="55">
+    <row r="113" spans="1:11" s="255" customFormat="1" ht="24">
       <c r="A113" s="9"/>
       <c r="B113" s="15">
         <v>24899714</v>
@@ -35606,7 +35671,7 @@
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
     </row>
-    <row r="117" spans="1:11" ht="44">
+    <row r="117" spans="1:11" ht="36">
       <c r="B117" s="79">
         <v>25009276</v>
       </c>
@@ -35632,7 +35697,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="118" spans="1:11" s="255" customFormat="1" ht="24">
+    <row r="118" spans="1:11" s="255" customFormat="1" ht="26">
       <c r="A118" s="9"/>
       <c r="B118" s="10">
         <v>25031397</v>
@@ -35744,7 +35809,7 @@
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="1:11" ht="26">
+    <row r="122" spans="1:11" ht="36">
       <c r="B122" s="15">
         <v>25031405</v>
       </c>
@@ -35796,7 +35861,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="48">
+    <row r="124" spans="1:11" ht="24">
       <c r="B124" s="15">
         <v>25031405</v>
       </c>
@@ -35822,7 +35887,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="36">
+    <row r="125" spans="1:11" ht="24">
       <c r="B125" s="15">
         <v>25031405</v>
       </c>
@@ -35848,7 +35913,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="36">
+    <row r="126" spans="1:11" ht="24">
       <c r="B126" s="15">
         <v>25031405</v>
       </c>
@@ -35874,7 +35939,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="24">
+    <row r="127" spans="1:11" ht="36">
       <c r="B127" s="15">
         <v>25031405</v>
       </c>
@@ -35900,14 +35965,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="24">
+    <row r="128" spans="1:11" ht="26">
       <c r="B128" s="79">
         <v>25043553</v>
       </c>
       <c r="C128" s="132" t="s">
         <v>299</v>
       </c>
-      <c r="D128" s="324" t="s">
+      <c r="D128" s="319" t="s">
         <v>196</v>
       </c>
       <c r="E128" s="15" t="s">
@@ -35926,14 +35991,14 @@
         <v>198</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="24">
+    <row r="129" spans="1:11" ht="26">
       <c r="B129" s="79">
         <v>25043553</v>
       </c>
       <c r="C129" s="205" t="s">
         <v>25</v>
       </c>
-      <c r="D129" s="327" t="s">
+      <c r="D129" s="322" t="s">
         <v>1450</v>
       </c>
       <c r="E129" s="129" t="s">
@@ -35952,7 +36017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="36">
+    <row r="130" spans="1:11" ht="12">
       <c r="B130" s="15">
         <v>25080583</v>
       </c>
@@ -35980,7 +36045,7 @@
       <c r="J130" s="12"/>
       <c r="K130" s="12"/>
     </row>
-    <row r="131" spans="1:11" ht="26">
+    <row r="131" spans="1:11" ht="48">
       <c r="B131" s="15">
         <v>25100599</v>
       </c>
@@ -36008,7 +36073,7 @@
       <c r="J131" s="230"/>
       <c r="K131" s="12"/>
     </row>
-    <row r="132" spans="1:11" ht="26">
+    <row r="132" spans="1:11" ht="36">
       <c r="B132" s="15">
         <v>25100604</v>
       </c>
@@ -36036,7 +36101,7 @@
       <c r="J132" s="12"/>
       <c r="K132" s="12"/>
     </row>
-    <row r="133" spans="1:11" ht="12">
+    <row r="133" spans="1:11" ht="36">
       <c r="B133" s="15">
         <v>25100604</v>
       </c>
@@ -36064,7 +36129,7 @@
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
     </row>
-    <row r="134" spans="1:11" ht="39">
+    <row r="134" spans="1:11" ht="24">
       <c r="B134" s="15">
         <v>25100604</v>
       </c>
@@ -36120,7 +36185,7 @@
       <c r="J135" s="12"/>
       <c r="K135" s="12"/>
     </row>
-    <row r="136" spans="1:11" ht="36">
+    <row r="136" spans="1:11" ht="12">
       <c r="B136" s="15">
         <v>25100604</v>
       </c>
@@ -36179,7 +36244,7 @@
       <c r="J137" s="263"/>
       <c r="K137" s="263"/>
     </row>
-    <row r="138" spans="1:11" ht="24">
+    <row r="138" spans="1:11" ht="12">
       <c r="A138" s="255" t="s">
         <v>1489</v>
       </c>
@@ -36192,19 +36257,19 @@
       <c r="D138" s="255" t="s">
         <v>1491</v>
       </c>
-      <c r="E138" s="328" t="s">
-        <v>3</v>
-      </c>
-      <c r="F138" s="328" t="s">
-        <v>1389</v>
-      </c>
-      <c r="G138" s="328" t="s">
+      <c r="E138" s="323" t="s">
+        <v>3</v>
+      </c>
+      <c r="F138" s="323" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G138" s="323" t="s">
         <v>3</v>
       </c>
       <c r="H138" s="258" t="s">
         <v>7</v>
       </c>
-      <c r="I138" s="328" t="s">
+      <c r="I138" s="323" t="s">
         <v>3</v>
       </c>
       <c r="J138" s="273"/>
@@ -36223,10 +36288,10 @@
       <c r="D139" s="255" t="s">
         <v>1492</v>
       </c>
-      <c r="E139" s="328" t="s">
-        <v>3</v>
-      </c>
-      <c r="F139" s="328" t="s">
+      <c r="E139" s="323" t="s">
+        <v>3</v>
+      </c>
+      <c r="F139" s="323" t="s">
         <v>1389</v>
       </c>
       <c r="G139" s="258" t="s">
@@ -36235,7 +36300,7 @@
       <c r="H139" s="258" t="s">
         <v>3</v>
       </c>
-      <c r="I139" s="328" t="s">
+      <c r="I139" s="323" t="s">
         <v>3</v>
       </c>
       <c r="J139" s="273"/>
@@ -36263,7 +36328,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="141" spans="1:11" s="255" customFormat="1" ht="12">
+    <row r="141" spans="1:11" s="255" customFormat="1" ht="24">
       <c r="A141" s="9"/>
       <c r="B141" s="224">
         <v>24899714</v>
@@ -36288,14 +36353,14 @@
       <c r="J141" s="10"/>
       <c r="K141" s="10"/>
     </row>
-    <row r="142" spans="1:11" s="255" customFormat="1" ht="12">
+    <row r="142" spans="1:11" s="255" customFormat="1" ht="55">
       <c r="A142" s="259" t="s">
         <v>1481</v>
       </c>
-      <c r="B142" s="322">
+      <c r="B142" s="317">
         <v>24920622</v>
       </c>
-      <c r="C142" s="322" t="s">
+      <c r="C142" s="317" t="s">
         <v>358</v>
       </c>
       <c r="D142" s="257" t="s">
@@ -36315,14 +36380,14 @@
       <c r="J142" s="263"/>
       <c r="K142" s="263"/>
     </row>
-    <row r="143" spans="1:11" s="255" customFormat="1" ht="12">
+    <row r="143" spans="1:11" s="255" customFormat="1" ht="13">
       <c r="A143" s="255" t="s">
         <v>1487</v>
       </c>
       <c r="B143" s="273">
         <v>25031397</v>
       </c>
-      <c r="C143" s="323"/>
+      <c r="C143" s="318"/>
       <c r="D143" s="264" t="s">
         <v>1486</v>
       </c>
@@ -39007,9 +39072,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W929"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -39097,7 +39162,7 @@
       </c>
       <c r="J2" s="7">
         <f>COUNTIF(J4:J594,"y")/COUNTA(J4:J594)</f>
-        <v>0.85</v>
+        <v>0.84158415841584155</v>
       </c>
       <c r="K2" s="40"/>
       <c r="L2" s="40"/>
@@ -39107,7 +39172,7 @@
       </c>
       <c r="N2" s="40">
         <f>COUNTA(J4:J104)</f>
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="9" customFormat="1" ht="13">
@@ -39158,7 +39223,9 @@
       <c r="I4" s="129" t="s">
         <v>1393</v>
       </c>
-      <c r="J4" s="15"/>
+      <c r="J4" s="129" t="s">
+        <v>7</v>
+      </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -45262,8 +45329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -45324,7 +45391,7 @@
       </c>
       <c r="D4" s="94">
         <f>B14</f>
-        <v>0.85</v>
+        <v>0.84158415841584155</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15">
@@ -45460,11 +45527,11 @@
       </c>
       <c r="B14" s="102">
         <f>D14/C14</f>
-        <v>0.85</v>
+        <v>0.84158415841584155</v>
       </c>
       <c r="C14" s="103">
         <f>'Software- POST C v NC'!N2</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D14" s="103">
         <f>'Software- POST C v NC'!M2</f>
@@ -45520,18 +45587,18 @@
         <v>0.96137339055793991</v>
       </c>
       <c r="C18" s="32">
-        <v>0.97623000000000004</v>
+        <v>0.97965000000000002</v>
       </c>
       <c r="D18" s="32">
-        <v>0.93779000000000001</v>
+        <v>0.93964000000000003</v>
       </c>
       <c r="E18" s="22">
         <f>ABS(B18-D18)</f>
-        <v>2.3583390557939898E-2</v>
+        <v>2.173339055793988E-2</v>
       </c>
       <c r="F18" s="23">
         <f>ABS(B18-C18)</f>
-        <v>1.4856609442060131E-2</v>
+        <v>1.827660944206011E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -45583,18 +45650,18 @@
         <v>0.82014388489208634</v>
       </c>
       <c r="C21" s="32">
-        <v>0.87643000000000004</v>
+        <v>0.88009000000000004</v>
       </c>
       <c r="D21" s="32">
-        <v>0.73889000000000005</v>
+        <v>0.74604999999999999</v>
       </c>
       <c r="E21" s="22">
         <f>ABS(B21-D21)</f>
-        <v>8.1253884892086292E-2</v>
+        <v>7.4093884892086348E-2</v>
       </c>
       <c r="F21" s="23">
         <f>ABS(B21-C21)</f>
-        <v>5.6286115107913703E-2</v>
+        <v>5.99461151079137E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -45643,21 +45710,21 @@
       </c>
       <c r="B24" s="112">
         <f>B14</f>
-        <v>0.85</v>
+        <v>0.84158415841584155</v>
       </c>
       <c r="C24" s="153">
-        <v>0.92744000000000004</v>
+        <v>0.90664999999999996</v>
       </c>
       <c r="D24" s="153">
-        <v>0.78385000000000005</v>
+        <v>0.75553000000000003</v>
       </c>
       <c r="E24" s="22">
         <f>ABS(B24-0.66874)</f>
-        <v>0.18125999999999998</v>
+        <v>0.17284415841584155</v>
       </c>
       <c r="F24" s="23">
         <f>ABS(B24-C24)</f>
-        <v>7.7440000000000064E-2</v>
+        <v>6.5065841584158401E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -45667,16 +45734,16 @@
     </row>
     <row r="26" spans="1:6" s="9" customFormat="1"/>
     <row r="27" spans="1:6">
-      <c r="A27" s="303" t="s">
+      <c r="A27" s="324" t="s">
         <v>958</v>
       </c>
-      <c r="B27" s="303"/>
-      <c r="C27" s="303"/>
-      <c r="D27" s="304" t="s">
+      <c r="B27" s="324"/>
+      <c r="C27" s="324"/>
+      <c r="D27" s="325" t="s">
         <v>959</v>
       </c>
-      <c r="E27" s="305"/>
-      <c r="F27" s="305"/>
+      <c r="E27" s="326"/>
+      <c r="F27" s="326"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
@@ -45715,11 +45782,11 @@
       </c>
       <c r="E29" s="27">
         <f>E18</f>
-        <v>2.3583390557939898E-2</v>
+        <v>2.173339055793988E-2</v>
       </c>
       <c r="F29" s="31">
         <f>F18</f>
-        <v>1.4856609442060131E-2</v>
+        <v>1.827660944206011E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -45739,11 +45806,11 @@
       </c>
       <c r="E30" s="27">
         <f>E21</f>
-        <v>8.1253884892086292E-2</v>
+        <v>7.4093884892086348E-2</v>
       </c>
       <c r="F30" s="31">
         <f>F21</f>
-        <v>5.6286115107913703E-2</v>
+        <v>5.99461151079137E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -45763,11 +45830,11 @@
       </c>
       <c r="E31" s="22">
         <f>E24</f>
-        <v>0.18125999999999998</v>
+        <v>0.17284415841584155</v>
       </c>
       <c r="F31" s="23">
         <f>F24</f>
-        <v>7.7440000000000064E-2</v>
+        <v>6.5065841584158401E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="24">
@@ -45787,11 +45854,11 @@
       </c>
       <c r="B34" s="16">
         <f>'binary significance test'!E12</f>
-        <v>-11.423058736627631</v>
+        <v>-10.921522173458614</v>
       </c>
       <c r="C34" s="16">
         <f>ABS(B34)</f>
-        <v>11.423058736627631</v>
+        <v>10.921522173458614</v>
       </c>
       <c r="D34" t="str">
         <f>IF(C34&gt;1.96,"y")</f>
@@ -45804,11 +45871,11 @@
       </c>
       <c r="B35" s="16">
         <f>'binary significance test'!I12</f>
-        <v>-3.0578435384838656</v>
+        <v>-3.2263431262954181</v>
       </c>
       <c r="C35" s="16">
         <f>ABS(B35)</f>
-        <v>3.0578435384838656</v>
+        <v>3.2263431262954181</v>
       </c>
       <c r="D35" t="str">
         <f>IF(C35&gt;1.96,"y")</f>
@@ -45821,11 +45888,11 @@
       </c>
       <c r="B36" s="16">
         <f>'binary significance test'!M12</f>
-        <v>-4.723743702524307</v>
+        <v>-4.2997883072518217</v>
       </c>
       <c r="C36" s="16">
         <f>ABS(B36)</f>
-        <v>4.723743702524307</v>
+        <v>4.2997883072518217</v>
       </c>
       <c r="D36" t="str">
         <f>IF(C36&gt;1.96,"y")</f>
@@ -45858,7 +45925,7 @@
   <dimension ref="B3:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -45877,23 +45944,23 @@
     </row>
     <row r="4" spans="2:13" ht="15">
       <c r="B4" s="44"/>
-      <c r="C4" s="306" t="s">
+      <c r="C4" s="327" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="306"/>
-      <c r="E4" s="306"/>
-      <c r="F4" s="306" t="s">
+      <c r="D4" s="327"/>
+      <c r="E4" s="327"/>
+      <c r="F4" s="327" t="s">
         <v>1347</v>
       </c>
-      <c r="G4" s="306"/>
-      <c r="H4" s="306"/>
-      <c r="I4" s="306"/>
-      <c r="J4" s="306" t="s">
+      <c r="G4" s="327"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="306"/>
-      <c r="L4" s="306"/>
-      <c r="M4" s="306"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
+      <c r="M4" s="327"/>
     </row>
     <row r="5" spans="2:13" ht="16">
       <c r="C5" s="42" t="s">
@@ -45932,7 +45999,7 @@
         <v>1333</v>
       </c>
       <c r="E6" s="46">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="G6" s="42" t="s">
         <v>1332</v>
@@ -45941,7 +46008,7 @@
         <v>1333</v>
       </c>
       <c r="I6" s="46">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="K6" s="42" t="s">
         <v>1332</v>
@@ -45950,7 +46017,7 @@
         <v>1333</v>
       </c>
       <c r="M6" s="46">
-        <v>0.87</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="16">
@@ -45990,7 +46057,7 @@
         <v>1337</v>
       </c>
       <c r="E8" s="46">
-        <v>434</v>
+        <v>466</v>
       </c>
       <c r="G8" s="42" t="s">
         <v>1336</v>
@@ -45999,7 +46066,7 @@
         <v>1337</v>
       </c>
       <c r="I8" s="46">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>1336</v>
@@ -46008,7 +46075,7 @@
         <v>1337</v>
       </c>
       <c r="M8" s="46">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -46036,7 +46103,7 @@
       </c>
       <c r="E11" s="48">
         <f>AVERAGE(E5:E6)</f>
-        <v>0.73499999999999999</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>1338</v>
@@ -46046,7 +46113,7 @@
       </c>
       <c r="I11" s="48">
         <f>AVERAGE(I5:I6)</f>
-        <v>0.7</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>1338</v>
@@ -46056,7 +46123,7 @@
       </c>
       <c r="M11" s="48">
         <f>AVERAGE(M5:M6)</f>
-        <v>0.69</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="16">
@@ -46068,7 +46135,7 @@
       </c>
       <c r="E12" s="49">
         <f>(E5-E6)/(SQRT(E11*(1-E11)*((1/E7)+(1/E8))))</f>
-        <v>-11.423058736627631</v>
+        <v>-10.921522173458614</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>1340</v>
@@ -46078,7 +46145,7 @@
       </c>
       <c r="I12" s="49">
         <f>(I5-I6)/(SQRT(I11*(1-I11)*((1/I7)+(1/I8))))</f>
-        <v>-3.0578435384838656</v>
+        <v>-3.2263431262954181</v>
       </c>
       <c r="K12" s="42" t="s">
         <v>1340</v>
@@ -46088,45 +46155,45 @@
       </c>
       <c r="M12" s="49">
         <f>(M5-M6)/(SQRT(M11*(1-M11)*((1/M7)+(1/M8))))</f>
-        <v>-4.723743702524307</v>
+        <v>-4.2997883072518217</v>
       </c>
     </row>
     <row r="14" spans="2:13">
-      <c r="C14" s="307" t="s">
+      <c r="C14" s="328" t="s">
         <v>1342</v>
       </c>
-      <c r="D14" s="307"/>
-      <c r="E14" s="307"/>
-      <c r="F14" s="307"/>
-      <c r="G14" s="307"/>
+      <c r="D14" s="328"/>
+      <c r="E14" s="328"/>
+      <c r="F14" s="328"/>
+      <c r="G14" s="328"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="C15" s="307"/>
-      <c r="D15" s="307"/>
-      <c r="E15" s="307"/>
-      <c r="F15" s="307"/>
-      <c r="G15" s="307"/>
+      <c r="C15" s="328"/>
+      <c r="D15" s="328"/>
+      <c r="E15" s="328"/>
+      <c r="F15" s="328"/>
+      <c r="G15" s="328"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="C16" s="307"/>
-      <c r="D16" s="307"/>
-      <c r="E16" s="307"/>
-      <c r="F16" s="307"/>
-      <c r="G16" s="307"/>
+      <c r="C16" s="328"/>
+      <c r="D16" s="328"/>
+      <c r="E16" s="328"/>
+      <c r="F16" s="328"/>
+      <c r="G16" s="328"/>
     </row>
     <row r="17" spans="3:7">
-      <c r="C17" s="307"/>
-      <c r="D17" s="307"/>
-      <c r="E17" s="307"/>
-      <c r="F17" s="307"/>
-      <c r="G17" s="307"/>
+      <c r="C17" s="328"/>
+      <c r="D17" s="328"/>
+      <c r="E17" s="328"/>
+      <c r="F17" s="328"/>
+      <c r="G17" s="328"/>
     </row>
     <row r="18" spans="3:7">
-      <c r="C18" s="307"/>
-      <c r="D18" s="307"/>
-      <c r="E18" s="307"/>
-      <c r="F18" s="307"/>
-      <c r="G18" s="307"/>
+      <c r="C18" s="328"/>
+      <c r="D18" s="328"/>
+      <c r="E18" s="328"/>
+      <c r="F18" s="328"/>
+      <c r="G18" s="328"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>